<commit_message>
update file import excel terbaru
</commit_message>
<xml_diff>
--- a/public/sampleBB.xlsx
+++ b/public/sampleBB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp_8\htdocs\coba_newitportal\IT-PORTAL-HO\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAB97EE-C3C6-4307-9208-769128BCD43C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC2E1F9-91F5-4804-8C4A-AADDF92924A1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AA518A1B-D065-49A0-8AFF-0FB34B05899E}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>note</t>
   </si>
   <si>
-    <t>FORMAT IMPORT DATA ACCESS POINT (PADA COLUMN MAX_ID WAJIB DI ISI NOMER URUT SESUAI DENGAN NOMER URUT INVENTORY)</t>
-  </si>
-  <si>
     <t>Ubiquiti</t>
   </si>
   <si>
@@ -157,6 +154,9 @@
   </si>
   <si>
     <t>PPAHOBB003</t>
+  </si>
+  <si>
+    <t>FORMAT IMPORT DATA WIRELLESS (PADA COLUMN MAX_ID WAJIB DI ISI NOMER URUT SESUAI DENGAN NOMER URUT INVENTORY)</t>
   </si>
 </sst>
 </file>
@@ -714,7 +714,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -917,7 +917,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -949,7 +949,7 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="16" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
@@ -966,13 +966,13 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>1</v>
@@ -987,7 +987,7 @@
         <v>4</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>5</v>
@@ -996,7 +996,7 @@
         <v>6</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>7</v>
@@ -1013,43 +1013,43 @@
         <v>1</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="10">
         <v>1232</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E17" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K17" s="3" t="s">
+      <c r="L17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="N17" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="N17" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -1057,43 +1057,43 @@
         <v>2</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="10">
         <v>10212</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E18" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="3" t="s">
+      <c r="L18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N18" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="N18" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -1101,43 +1101,43 @@
         <v>3</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="10">
         <v>11202</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E19" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="L19" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update formatted import inventory
</commit_message>
<xml_diff>
--- a/public/sampleBB.xlsx
+++ b/public/sampleBB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT PPA-BIB\Documents\PROJECT ICT SOFTWARE\IT-PORTAL-HO-FIXED-ONLY-HO\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{06A8A337-5407-47ED-A31F-93DD6C8AC4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA43EF78-2ACE-46BD-A19C-BEC5B175B683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AA518A1B-D065-49A0-8AFF-0FB34B05899E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{AA518A1B-D065-49A0-8AFF-0FB34B05899E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t>device_name</t>
   </si>
@@ -66,27 +66,15 @@
     <t>Asset Ho Number</t>
   </si>
   <si>
-    <t>LIST DATA IMPORT AP &amp; Panduan Pengisian</t>
-  </si>
-  <si>
     <t xml:space="preserve">* KOLOM/DATA TIDAK BOLOEH KOSONG, JIKA ADA YANG KOSONG MAKA DI ISIKAN DENGAN (-) </t>
   </si>
   <si>
     <t>* PENGISIAN NOMER INVENTORY SESUAIKAN DENGAN SITE MASING MASING, UNTUK DATA YANG SUDAH ADA PADA SHEET INI BOLEH DI HAPUS KARENA HANYA BERSIFAT SAMPLE DATA!</t>
   </si>
   <si>
-    <t>* UNTUK DEVICE DENGAN MERK UBUQUITY MAKA SN NYA ISI DENGAN MAC ADDRESS SESUAI AKTUAL DATA, JIKA MERK BUKAN UBIQUITY MAKA ISI DENGAN SESUAI DATA AKTUAL YANG ADA PADA SITE MASING-MASING</t>
-  </si>
-  <si>
-    <t>* PADA BAGIAN KOLOM FREQUENCY ISIKAN DENGAN FREQUESNCY YANG SEDANG DI GUNAKAN/ DI PANCARKAN OLEH DEVICE TERSEBUT SECARA AKTUAL</t>
-  </si>
-  <si>
     <t>5.8 Ghz</t>
   </si>
   <si>
-    <t>* PADA BAGIAN KOLONG DEVICE MODEL ISIKAN DENGAN AKTUAL FREQUENCY YANG BISA DI GUNAKAN OLEH DEVICE TERSEBUT, JIKA BISA 2,4 /5.8 GHZ MAKA ISI DENGAN AKTUAL, JIKA ONLY 5.8 GHZ MAKA ISI DENGAN AKTUALNYA 5.8 GHZ SAJA</t>
-  </si>
-  <si>
     <t>DIMOHON UNTUK MEMBACA PETUNJUK DI ATAS SEBELUM MELAKUKAN PENGISIAN DATA, UNTUK MENGHINDARI ADANYA KESALAHAN/GAGAL IMPORT DATA PADA SISTEM.</t>
   </si>
   <si>
@@ -172,6 +160,15 @@
   </si>
   <si>
     <t>SCRAP</t>
+  </si>
+  <si>
+    <t>LIST DATA IMPORT BB/WIRELLESS &amp; Panduan Pengisian</t>
+  </si>
+  <si>
+    <t>* PADA BAGIAN KOLOM FREQUENCY ISIKAN DENGAN FREQUENCY YANG SEDANG DI GUNAKAN/ DI PANCARKAN OLEH DEVICE TERSEBUT SECARA AKTUAL</t>
+  </si>
+  <si>
+    <t>* PADA BAGIAN KOLOM DEVICE MODEL ISIKAN DENGAN AKTUAL DARI MODEL BACKBONE/WIRELLESS</t>
   </si>
 </sst>
 </file>
@@ -314,7 +311,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -325,20 +322,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -351,6 +336,19 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
@@ -689,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C41EB6C-1614-4483-BF76-7A2D3A426679}">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
-      <selection activeCell="E25" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -712,42 +710,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="A1" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -765,7 +763,7 @@
     </row>
     <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -782,8 +780,8 @@
       <c r="N4" s="2"/>
     </row>
     <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>16</v>
+      <c r="A5" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="3"/>
@@ -800,8 +798,8 @@
       <c r="N5" s="2"/>
     </row>
     <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>17</v>
+      <c r="A6" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -818,9 +816,7 @@
       <c r="N6" s="5"/>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="A7" s="16"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -900,38 +896,38 @@
       <c r="N11" s="2"/>
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
+      <c r="A12" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
     </row>
     <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
     </row>
     <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
@@ -966,46 +962,46 @@
       <c r="N15" s="5"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="8" t="s">
+      <c r="A16" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H16" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="12" t="s">
+      <c r="H16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J16" s="12" t="s">
+      <c r="J16" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="K16" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="L16" s="12" t="s">
+      <c r="K16" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L16" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="M16" s="12" t="s">
+      <c r="M16" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="N16" s="12" t="s">
+      <c r="N16" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1014,43 +1010,43 @@
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="9">
+        <v>1232</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C17" s="13">
-        <v>1232</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N17" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
@@ -1058,43 +1054,43 @@
         <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="13">
+        <v>20</v>
+      </c>
+      <c r="C18" s="9">
         <v>10212</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>11</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
@@ -1102,43 +1098,43 @@
         <v>3</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="13">
+        <v>20</v>
+      </c>
+      <c r="C19" s="9">
         <v>11202</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>43</v>
+        <v>38</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>10</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>